<commit_message>
v1.0.0 -rev(b) Adding RCD Edits v1 and v2.
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-DispenseRefill.xlsx
+++ b/output/StructureDefinition-DispenseRefill.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$6</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="68">
   <si>
     <t>Path</t>
   </si>
@@ -173,23 +173,10 @@
     <t>Extension.extension</t>
   </si>
   <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
     <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
     <t xml:space="preserve">value:url}
 </t>
   </si>
@@ -203,19 +190,7 @@
     <t>Element.extension</t>
   </si>
   <si>
-    <t>refillNum</t>
-  </si>
-  <si>
-    <t>Refill number of this prescription</t>
-  </si>
-  <si>
-    <t>Extension.extension.id</t>
-  </si>
-  <si>
-    <t>Extension.extension.extension</t>
-  </si>
-  <si>
-    <t>Extension.extension.url</t>
+    <t>Extension.url</t>
   </si>
   <si>
     <t xml:space="preserve">uri
@@ -231,47 +206,27 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>Extension.url</t>
+    <t>http://hl7.org/fhir/us/davinci-pdex/StructureDefinition/DispenseRefill</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Extension.extension.value[x]</t>
+    <t>Extension.value[x]</t>
   </si>
   <si>
     <t xml:space="preserve">Quantity
 </t>
   </si>
   <si>
-    <t>Value of extension</t>
+    <t>Refill number of this prescription</t>
   </si>
   <si>
     <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R4/extensibility.html) for a list).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
-    <t>Extension.value[x]</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
-  </si>
-  <si>
-    <t>valueQuantity</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-pdex/StructureDefinition/DispenseRefill</t>
-  </si>
-  <si>
-    <t>base64Binary
-booleancanonicalcodedatedateTimedecimalidinstantintegermarkdownoidpositiveIntstringtimeunsignedInturiurluuidAddressAgeAnnotationAttachmentCodeableConceptCodingContactPointCountDistanceDurationHumanNameIdentifierMoneyPeriodQuantityRangeRatioReferenceSampledDataSignatureTimingContactDetailContributorDataRequirementExpressionParameterDefinitionRelatedArtifactTriggerDefinitionUsageContextDosageMeta</t>
   </si>
 </sst>
 </file>
@@ -420,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ12"/>
+  <dimension ref="A1:AJ6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -429,9 +384,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="29.53515625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="14.23046875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.91015625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="1" max="1" width="19.89453125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.16796875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
@@ -439,7 +394,7 @@
     <col min="8" max="8" width="12.07421875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="45.53125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="38.6796875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -783,14 +738,14 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
         <v>38</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s" s="2">
         <v>37</v>
@@ -802,17 +757,15 @@
         <v>37</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="M4" t="s" s="2">
-        <v>55</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
         <v>37</v>
@@ -849,19 +802,19 @@
         <v>37</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AC4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>38</v>
@@ -876,22 +829,20 @@
         <v>42</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>60</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s" s="2">
         <v>44</v>
@@ -906,22 +857,24 @@
         <v>37</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="M5" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="M5" t="s" s="2">
+        <v>60</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
         <v>37</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s" s="2">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="R5" t="s" s="2">
         <v>37</v>
@@ -963,27 +916,27 @@
         <v>37</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1006,13 +959,13 @@
         <v>37</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1063,7 +1016,7 @@
         <v>37</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>38</v>
@@ -1075,618 +1028,14 @@
         <v>37</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" hidden="true">
-      <c r="A7" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="G7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J7" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="K7" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="L7" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="R7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA7" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AB7" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="AC7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD7" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AE7" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AF7" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG7" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AH7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI7" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ7" t="s" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" hidden="true">
-      <c r="A8" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F8" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J8" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="K8" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="L8" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="M8" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="R8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE8" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="AF8" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG8" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AJ8" t="s" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" hidden="true">
-      <c r="A9" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J9" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="K9" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="L9" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P9" s="2"/>
-      <c r="Q9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="R9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA9" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB9" s="2"/>
-      <c r="AC9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD9" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE9" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF9" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG9" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI9" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AJ9" t="s" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" hidden="true">
-      <c r="A10" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="F10" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J10" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="K10" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="L10" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P10" s="2"/>
-      <c r="Q10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="R10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE10" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF10" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG10" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI10" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AJ10" t="s" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" hidden="true">
-      <c r="A11" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J11" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="K11" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="L11" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="N11" s="2"/>
-      <c r="O11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="R11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE11" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="AF11" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG11" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AJ11" t="s" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" hidden="true">
-      <c r="A12" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="F12" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="G12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J12" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="K12" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="L12" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="R12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE12" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF12" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG12" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AJ12" t="s" s="2">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ12">
+  <autoFilter ref="A1:AJ6">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -1696,7 +1045,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI11">
+  <conditionalFormatting sqref="A2:AI5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
add profile and vocab files
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-DispenseRefill.xlsx
+++ b/output/StructureDefinition-DispenseRefill.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$6</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="68">
   <si>
     <t>Path</t>
   </si>
@@ -173,23 +173,10 @@
     <t>Extension.extension</t>
   </si>
   <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
     <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
     <t xml:space="preserve">value:url}
 </t>
   </si>
@@ -203,19 +190,7 @@
     <t>Element.extension</t>
   </si>
   <si>
-    <t>refillNum</t>
-  </si>
-  <si>
-    <t>Refill number of this prescription</t>
-  </si>
-  <si>
-    <t>Extension.extension.id</t>
-  </si>
-  <si>
-    <t>Extension.extension.extension</t>
-  </si>
-  <si>
-    <t>Extension.extension.url</t>
+    <t>Extension.url</t>
   </si>
   <si>
     <t xml:space="preserve">uri
@@ -231,47 +206,27 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>Extension.url</t>
+    <t>http://hl7.org/fhir/us/davinci-pdex/StructureDefinition/DispenseRefill</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Extension.extension.value[x]</t>
+    <t>Extension.value[x]</t>
   </si>
   <si>
     <t xml:space="preserve">Quantity
 </t>
   </si>
   <si>
-    <t>Value of extension</t>
+    <t>Refill number of this prescription</t>
   </si>
   <si>
     <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R4/extensibility.html) for a list).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
-    <t>Extension.value[x]</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
-  </si>
-  <si>
-    <t>valueQuantity</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-pdex/StructureDefinition/DispenseRefill</t>
-  </si>
-  <si>
-    <t>base64Binary
-booleancanonicalcodedatedateTimedecimalidinstantintegermarkdownoidpositiveIntstringtimeunsignedInturiurluuidAddressAgeAnnotationAttachmentCodeableConceptCodingContactPointCountDistanceDurationHumanNameIdentifierMoneyPeriodQuantityRangeRatioReferenceSampledDataSignatureTimingContactDetailContributorDataRequirementExpressionParameterDefinitionRelatedArtifactTriggerDefinitionUsageContextDosageMeta</t>
   </si>
 </sst>
 </file>
@@ -420,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ12"/>
+  <dimension ref="A1:AJ6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -429,9 +384,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="29.53515625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="14.23046875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.91015625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="1" max="1" width="19.89453125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.16796875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
@@ -439,7 +394,7 @@
     <col min="8" max="8" width="12.07421875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="45.53125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="38.6796875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -783,14 +738,14 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
         <v>38</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s" s="2">
         <v>37</v>
@@ -802,17 +757,15 @@
         <v>37</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="M4" t="s" s="2">
-        <v>55</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
         <v>37</v>
@@ -849,19 +802,19 @@
         <v>37</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AC4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>38</v>
@@ -876,22 +829,20 @@
         <v>42</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>60</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s" s="2">
         <v>44</v>
@@ -906,22 +857,24 @@
         <v>37</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="M5" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="M5" t="s" s="2">
+        <v>60</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
         <v>37</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s" s="2">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="R5" t="s" s="2">
         <v>37</v>
@@ -963,27 +916,27 @@
         <v>37</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1006,13 +959,13 @@
         <v>37</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1063,7 +1016,7 @@
         <v>37</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>38</v>
@@ -1075,618 +1028,14 @@
         <v>37</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" hidden="true">
-      <c r="A7" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="G7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J7" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="K7" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="L7" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="R7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA7" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AB7" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="AC7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD7" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AE7" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AF7" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG7" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AH7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI7" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ7" t="s" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" hidden="true">
-      <c r="A8" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F8" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J8" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="K8" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="L8" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="M8" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="R8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE8" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="AF8" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG8" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AJ8" t="s" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" hidden="true">
-      <c r="A9" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J9" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="K9" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="L9" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P9" s="2"/>
-      <c r="Q9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="R9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA9" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB9" s="2"/>
-      <c r="AC9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD9" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE9" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF9" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG9" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI9" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AJ9" t="s" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" hidden="true">
-      <c r="A10" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="F10" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J10" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="K10" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="L10" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P10" s="2"/>
-      <c r="Q10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="R10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE10" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF10" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG10" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH10" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI10" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AJ10" t="s" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" hidden="true">
-      <c r="A11" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J11" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="K11" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="L11" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="N11" s="2"/>
-      <c r="O11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="R11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE11" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="AF11" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG11" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AJ11" t="s" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" hidden="true">
-      <c r="A12" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="F12" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="G12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J12" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="K12" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="L12" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="R12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE12" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF12" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG12" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI12" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AJ12" t="s" s="2">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ12">
+  <autoFilter ref="A1:AJ6">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -1696,7 +1045,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI11">
+  <conditionalFormatting sqref="A2:AI5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>